<commit_message>
Blog con APP_revisando AVATAR
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyctoFinalBlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0598399-FBAB-404F-8BCE-2AB10D060181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665FC136-032C-4C62-B69C-EDFAEDA21E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -77,30 +77,12 @@
     <t>Caso #1</t>
   </si>
   <si>
-    <t>listado de estudiantes</t>
-  </si>
-  <si>
-    <t>tlksdj</t>
-  </si>
-  <si>
     <t>Caso #2</t>
   </si>
   <si>
-    <t>agregarProfesor</t>
-  </si>
-  <si>
-    <t>cuando abro la vista de agregar profesor, debe aparecer un formuulario que me permita cargar profesores</t>
-  </si>
-  <si>
     <t>Caso #3</t>
   </si>
   <si>
-    <t>inicio</t>
-  </si>
-  <si>
-    <t>cuando cargo el inicio de la aplicacion, me debe mostrar una bienvenida y el logo de mi proyecto</t>
-  </si>
-  <si>
     <t>Ayudanos a Ayudarte</t>
   </si>
   <si>
@@ -113,17 +95,107 @@
     <t>Instalación de Boostrap, descargamos el Componente NAVBar, Card</t>
   </si>
   <si>
-    <t>Error en {% for post in post %}</t>
-  </si>
-  <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>En posts_page: Error en {% for post in post %}</t>
+  </si>
+  <si>
+    <t>Con ayuda de Coder Ask solucionamos el Error en {% for post in post %}</t>
+  </si>
+  <si>
+    <t>En TemplateDoesNotExist at /buscarBlog/ busquedaBlog.html</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Caso #4</t>
+  </si>
+  <si>
+    <t>En home page agregue un botón de acceso rápido a las búsquedas de Blogs</t>
+  </si>
+  <si>
+    <t>Problema al no cargar una imagen de portada</t>
+  </si>
+  <si>
+    <t>Se soluciono poniendo por default = "default-image.png"</t>
+  </si>
+  <si>
+    <t>Caso #5</t>
+  </si>
+  <si>
+    <t>Error al realizar la búsqueda de un Blog ---&gt; dos errores en la línea 93 de views.py ---&gt; Se Soluciono con: nombre=Post.objects.filter(title__icontains = nombre)</t>
+  </si>
+  <si>
+    <t>Caso #6</t>
+  </si>
+  <si>
+    <t>resultadoBusquedaBlog.html --&gt; arroja la búsqueda como TABLA</t>
+  </si>
+  <si>
+    <t>Se soluciono aplicando boostrap,css,js</t>
+  </si>
+  <si>
+    <t>Error al realizar la búsqueda de un Blog --&gt; colucionado redireccionando a resultadoBusquedaBlog.html</t>
+  </si>
+  <si>
+    <t>Problemas al crear la nueva APP Account para Register, Login, Logout, Editar Perfil</t>
+  </si>
+  <si>
+    <t>Caso #7</t>
+  </si>
+  <si>
+    <t>Revisamos con CoderAsk el día completo con 3 Tutores y no encuentran la falla</t>
+  </si>
+  <si>
+    <t>imagen_portada = models.ImageField(null=True, blank=True, default = 'default-image.png')</t>
+  </si>
+  <si>
+    <t>Caso #8</t>
+  </si>
+  <si>
+    <t>Había una imagen por defecto en el caso que el usuario no cargue una, por algún motivo ahora no aparece</t>
+  </si>
+  <si>
+    <t>Caso #9</t>
+  </si>
+  <si>
+    <t>Se creo el servicio de Mensajería sobre los Blogs</t>
+  </si>
+  <si>
+    <t>Me aparece el botón Comentar, sin embargo no me aparece el campo para dejar comentario</t>
+  </si>
+  <si>
+    <t>Caso #10</t>
+  </si>
+  <si>
+    <t>Estoy teniendo probelmas para subir al repo los commit, lo estamos revisndo con CoderAsk desde esta mañana. SIN SOLUCIÓN</t>
+  </si>
+  <si>
+    <t>Caso #11</t>
+  </si>
+  <si>
+    <t>Problemas con GITHUB</t>
+  </si>
+  <si>
+    <t>Se soluciono en "post.html" --&gt; poniendo &lt;p&gt; {{post.description|safe}} &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Problemas con el texto que se muestra en el contenido del Blog.</t>
+  </si>
+  <si>
+    <t>Caso #12</t>
+  </si>
+  <si>
+    <t>Problemas con el texto del servicio de Mensajería. No se muestran los comnetarios en los Blogs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,20 +207,44 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +261,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8EAADB"/>
         <bgColor rgb="FF8EAADB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -209,15 +299,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify"/>
@@ -228,14 +309,9 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,34 +528,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1000"/>
+  <dimension ref="A1:E996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
     <col min="4" max="4" width="61.42578125" customWidth="1"/>
     <col min="5" max="24" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -489,34 +565,34 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -533,172 +609,224 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8">
+        <v>45041</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8">
+        <v>45048</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="8">
+        <v>45048</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8">
+        <v>45049</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="13" t="s">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="8">
+        <v>45049</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>12</v>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="8">
+        <v>45049</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="10" t="s">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8">
+        <v>45049</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="8">
+        <v>45049</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="11">
-        <v>45041</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="11">
-        <v>45047</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>27</v>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="8">
+        <v>45050</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8">
+        <v>45050</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="8">
+        <v>45051</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="8">
+        <v>45051</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1663,11 +1791,11 @@
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:E19">
+    <sortCondition ref="D7:D19"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>